<commit_message>
Number of threads to parameter instead of define
</commit_message>
<xml_diff>
--- a/benchmark/benchmark_result_20160713.xlsx
+++ b/benchmark/benchmark_result_20160713.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Read config file:</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>2^30</t>
+  </si>
+  <si>
+    <t>cache:  3 MB</t>
+  </si>
+  <si>
+    <t>cores: 2</t>
+  </si>
+  <si>
+    <t>threads: 4</t>
   </si>
 </sst>
 </file>
@@ -230,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -253,12 +262,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -266,6 +284,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -551,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,6 +1252,21 @@
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>